<commit_message>
added data sources and simplified csv format
</commit_message>
<xml_diff>
--- a/lane_miles/lane_miles_data.xlsx
+++ b/lane_miles/lane_miles_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamb\Documents\projects\data vis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamb\Documents\projects\data_vis\lane_miles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{194F2150-3A1E-403C-90A4-FF08786BC4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EDD38E-8469-4FB2-BD2C-A4B87F45F0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D7D90053-7C6E-468C-8FFA-DDD58A1AC022}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
   <si>
     <t>Alabama</t>
   </si>
@@ -245,6 +245,33 @@
   </si>
   <si>
     <t>lane miles per person</t>
+  </si>
+  <si>
+    <t>data sources</t>
+  </si>
+  <si>
+    <t>https://www.fhwa.dot.gov/policyinformation/statistics/2020/hm60.cfm</t>
+  </si>
+  <si>
+    <t>road network data:</t>
+  </si>
+  <si>
+    <t>US Department of Transportation - Federal Highway Administration</t>
+  </si>
+  <si>
+    <t>population:</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_U.S._states_and_territories_by_population</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>land area:</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_U.S._states_and_territories_by_area</t>
   </si>
 </sst>
 </file>
@@ -252,10 +279,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="#,##0.000"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +309,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -412,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -432,24 +467,6 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -459,8 +476,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -469,6 +486,26 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,26 +820,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEF6F4E-8FB1-4CA9-89EE-8B722D924F6F}">
-  <dimension ref="A1:AI58"/>
+  <dimension ref="A1:AI59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y23" sqref="Y23"/>
+      <selection pane="bottomRight" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="13" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
@@ -812,112 +849,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="10" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11" t="s">
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="16"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="10"/>
     </row>
     <row r="2" spans="1:35" ht="57" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="12"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="16"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="10"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -971,33 +1008,33 @@
       <c r="Q3" s="1">
         <v>65461</v>
       </c>
-      <c r="R3" s="21">
+      <c r="R3" s="15">
         <v>209560</v>
       </c>
-      <c r="S3" s="22">
+      <c r="S3" s="16">
         <v>5039877</v>
       </c>
-      <c r="T3" s="20">
+      <c r="T3" s="14">
         <v>50645.33</v>
       </c>
-      <c r="U3" s="20">
+      <c r="U3" s="14">
         <f>S3/T3</f>
         <v>99.513163405194518</v>
       </c>
-      <c r="V3" s="18">
+      <c r="V3" s="12">
         <f>R3/T3</f>
         <v>4.1377951333321352</v>
       </c>
-      <c r="W3" s="19">
+      <c r="W3" s="13">
         <f>R3/S3</f>
         <v>4.1580379838634954E-2</v>
       </c>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="16"/>
-      <c r="AG3" s="16"/>
-      <c r="AI3" s="16"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AI3" s="10"/>
     </row>
     <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1051,33 +1088,33 @@
       <c r="Q4" s="1">
         <v>6802</v>
       </c>
-      <c r="R4" s="21">
+      <c r="R4" s="15">
         <v>35908</v>
       </c>
-      <c r="S4" s="22">
+      <c r="S4" s="16">
         <v>733391</v>
       </c>
-      <c r="T4" s="20">
+      <c r="T4" s="14">
         <v>570640.94999999995</v>
       </c>
-      <c r="U4" s="20">
+      <c r="U4" s="14">
         <f t="shared" ref="U4:U53" si="0">S4/T4</f>
         <v>1.2852056972076751</v>
       </c>
-      <c r="V4" s="18">
+      <c r="V4" s="12">
         <f t="shared" ref="V4:V53" si="1">R4/T4</f>
         <v>6.2925732897367428E-2</v>
       </c>
-      <c r="W4" s="19">
+      <c r="W4" s="13">
         <f t="shared" ref="W4:W54" si="2">R4/S4</f>
         <v>4.896160438292807E-2</v>
       </c>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AI4" s="16"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AI4" s="10"/>
     </row>
     <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1131,32 +1168,32 @@
       <c r="Q5" s="1">
         <v>62739</v>
       </c>
-      <c r="R5" s="21">
+      <c r="R5" s="15">
         <v>146761</v>
       </c>
-      <c r="S5" s="22">
+      <c r="S5" s="16">
         <v>7276316</v>
       </c>
-      <c r="T5" s="20">
+      <c r="T5" s="14">
         <v>113594.08</v>
       </c>
-      <c r="U5" s="20">
+      <c r="U5" s="14">
         <f t="shared" si="0"/>
         <v>64.055415563909662</v>
       </c>
-      <c r="V5" s="18">
+      <c r="V5" s="12">
         <f t="shared" si="1"/>
         <v>1.2919775396746027</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="13">
         <f t="shared" si="2"/>
         <v>2.0169684769050712E-2</v>
       </c>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1210,34 +1247,34 @@
       <c r="Q6" s="1">
         <v>37314</v>
       </c>
-      <c r="R6" s="21">
+      <c r="R6" s="15">
         <v>204105</v>
       </c>
-      <c r="S6" s="22">
+      <c r="S6" s="16">
         <v>3011524</v>
       </c>
-      <c r="T6" s="20">
+      <c r="T6" s="14">
         <v>52035.48</v>
       </c>
-      <c r="U6" s="20">
+      <c r="U6" s="14">
         <f t="shared" si="0"/>
         <v>57.874434904799571</v>
       </c>
-      <c r="V6" s="18">
+      <c r="V6" s="12">
         <f t="shared" si="1"/>
         <v>3.9224198566055311</v>
       </c>
-      <c r="W6" s="19">
+      <c r="W6" s="13">
         <f t="shared" si="2"/>
         <v>6.7774654958751776E-2</v>
       </c>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="16"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -1291,33 +1328,33 @@
       <c r="Q7" s="1">
         <v>243870</v>
       </c>
-      <c r="R7" s="21">
+      <c r="R7" s="15">
         <v>396616</v>
       </c>
-      <c r="S7" s="22">
+      <c r="S7" s="16">
         <v>39237836</v>
       </c>
-      <c r="T7" s="20">
+      <c r="T7" s="14">
         <v>155779.22</v>
       </c>
-      <c r="U7" s="20">
+      <c r="U7" s="14">
         <f t="shared" si="0"/>
         <v>251.88106603692071</v>
       </c>
-      <c r="V7" s="18">
+      <c r="V7" s="12">
         <f t="shared" si="1"/>
         <v>2.5460135183627188</v>
       </c>
-      <c r="W7" s="19">
+      <c r="W7" s="13">
         <f t="shared" si="2"/>
         <v>1.0107998820322303E-2</v>
       </c>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="15"/>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AI7" s="16"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AI7" s="10"/>
     </row>
     <row r="8" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1371,33 +1408,33 @@
       <c r="Q8" s="1">
         <v>47287</v>
       </c>
-      <c r="R8" s="21">
+      <c r="R8" s="15">
         <v>185827</v>
       </c>
-      <c r="S8" s="22">
+      <c r="S8" s="16">
         <v>5812069</v>
       </c>
-      <c r="T8" s="20">
+      <c r="T8" s="14">
         <v>103641.89</v>
       </c>
-      <c r="U8" s="20">
+      <c r="U8" s="14">
         <f t="shared" si="0"/>
         <v>56.078377188991823</v>
       </c>
-      <c r="V8" s="18">
+      <c r="V8" s="12">
         <f t="shared" si="1"/>
         <v>1.7929719344176376</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="13">
         <f t="shared" si="2"/>
         <v>3.1972607345164002E-2</v>
       </c>
-      <c r="AC8" s="15"/>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="15"/>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="16"/>
-      <c r="AI8" s="16"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AI8" s="10"/>
     </row>
     <row r="9" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -1451,34 +1488,34 @@
       <c r="Q9" s="1">
         <v>34334</v>
       </c>
-      <c r="R9" s="21">
+      <c r="R9" s="15">
         <v>45899</v>
       </c>
-      <c r="S9" s="22">
+      <c r="S9" s="16">
         <v>3605944</v>
       </c>
-      <c r="T9" s="20">
+      <c r="T9" s="14">
         <v>4842.3599999999997</v>
       </c>
-      <c r="U9" s="20">
+      <c r="U9" s="14">
         <f t="shared" si="0"/>
         <v>744.66665014579678</v>
       </c>
-      <c r="V9" s="18">
+      <c r="V9" s="12">
         <f t="shared" si="1"/>
         <v>9.4786426453217025</v>
       </c>
-      <c r="W9" s="19">
+      <c r="W9" s="13">
         <f t="shared" si="2"/>
         <v>1.2728705714786475E-2</v>
       </c>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="15"/>
-      <c r="AE9" s="15"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="16"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="10"/>
     </row>
     <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1532,35 +1569,35 @@
       <c r="Q10" s="1">
         <v>8174</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="15">
         <v>14119</v>
       </c>
-      <c r="S10" s="22">
+      <c r="S10" s="16">
         <v>989948</v>
       </c>
-      <c r="T10" s="20">
+      <c r="T10" s="14">
         <v>1948.54</v>
       </c>
-      <c r="U10" s="20">
+      <c r="U10" s="14">
         <f t="shared" si="0"/>
         <v>508.04602420273642</v>
       </c>
-      <c r="V10" s="18">
+      <c r="V10" s="12">
         <f t="shared" si="1"/>
         <v>7.2459379843369911</v>
       </c>
-      <c r="W10" s="19">
+      <c r="W10" s="13">
         <f t="shared" si="2"/>
         <v>1.4262365295954938E-2</v>
       </c>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="16"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="16"/>
-      <c r="AG10" s="16"/>
-      <c r="AI10" s="16"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="10"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AI10" s="10"/>
     </row>
     <row r="11" spans="1:35" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -1614,35 +1651,35 @@
       <c r="Q11" s="1">
         <v>3448</v>
       </c>
-      <c r="R11" s="21">
+      <c r="R11" s="15">
         <v>3448</v>
       </c>
-      <c r="S11" s="22">
+      <c r="S11" s="16">
         <v>689545</v>
       </c>
-      <c r="T11" s="20">
+      <c r="T11" s="14">
         <v>61.05</v>
       </c>
-      <c r="U11" s="20">
+      <c r="U11" s="14">
         <f t="shared" si="0"/>
         <v>11294.758394758395</v>
       </c>
-      <c r="V11" s="18">
+      <c r="V11" s="12">
         <f t="shared" si="1"/>
         <v>56.478296478296478</v>
       </c>
-      <c r="W11" s="19">
+      <c r="W11" s="13">
         <f t="shared" si="2"/>
         <v>5.0003988137104901E-3</v>
       </c>
-      <c r="Y11" s="16"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="15"/>
-      <c r="AF11" s="16"/>
-      <c r="AG11" s="16"/>
-      <c r="AH11" s="16"/>
-      <c r="AI11" s="16"/>
+      <c r="Y11" s="10"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="10"/>
+      <c r="AI11" s="10"/>
     </row>
     <row r="12" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1696,36 +1733,36 @@
       <c r="Q12" s="1">
         <v>198306</v>
       </c>
-      <c r="R12" s="21">
+      <c r="R12" s="15">
         <v>276289</v>
       </c>
-      <c r="S12" s="22">
+      <c r="S12" s="16">
         <v>21781128</v>
       </c>
-      <c r="T12" s="20">
+      <c r="T12" s="14">
         <v>53624.76</v>
       </c>
-      <c r="U12" s="20">
+      <c r="U12" s="14">
         <f t="shared" si="0"/>
         <v>406.17669897263875</v>
       </c>
-      <c r="V12" s="18">
+      <c r="V12" s="12">
         <f t="shared" si="1"/>
         <v>5.1522654833326991</v>
       </c>
-      <c r="W12" s="19">
+      <c r="W12" s="13">
         <f t="shared" si="2"/>
         <v>1.2684788409489169E-2</v>
       </c>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="16"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="17"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="16"/>
-      <c r="AG12" s="16"/>
-      <c r="AH12" s="16"/>
-      <c r="AI12" s="16"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="10"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="10"/>
     </row>
     <row r="13" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -1779,36 +1816,36 @@
       <c r="Q13" s="1">
         <v>115296</v>
       </c>
-      <c r="R13" s="21">
+      <c r="R13" s="15">
         <v>273086</v>
       </c>
-      <c r="S13" s="22">
+      <c r="S13" s="16">
         <v>10799566</v>
       </c>
-      <c r="T13" s="20">
+      <c r="T13" s="14">
         <v>57513.49</v>
       </c>
-      <c r="U13" s="20">
+      <c r="U13" s="14">
         <f t="shared" si="0"/>
         <v>187.77448560329066</v>
       </c>
-      <c r="V13" s="18">
+      <c r="V13" s="12">
         <f t="shared" si="1"/>
         <v>4.7482077682992285</v>
       </c>
-      <c r="W13" s="19">
+      <c r="W13" s="13">
         <f t="shared" si="2"/>
         <v>2.5286756893749249E-2</v>
       </c>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="16"/>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="15"/>
-      <c r="AF13" s="16"/>
-      <c r="AG13" s="16"/>
-      <c r="AH13" s="16"/>
-      <c r="AI13" s="16"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="10"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+      <c r="AH13" s="10"/>
+      <c r="AI13" s="10"/>
     </row>
     <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1862,36 +1899,36 @@
       <c r="Q14" s="1">
         <v>6485</v>
       </c>
-      <c r="R14" s="21">
+      <c r="R14" s="15">
         <v>9804</v>
       </c>
-      <c r="S14" s="22">
+      <c r="S14" s="16">
         <v>1455271</v>
       </c>
-      <c r="T14" s="20">
+      <c r="T14" s="14">
         <v>6422.63</v>
       </c>
-      <c r="U14" s="20">
+      <c r="U14" s="14">
         <f t="shared" si="0"/>
         <v>226.58490369210119</v>
       </c>
-      <c r="V14" s="18">
+      <c r="V14" s="12">
         <f t="shared" si="1"/>
         <v>1.5264774710671485</v>
       </c>
-      <c r="W14" s="19">
+      <c r="W14" s="13">
         <f t="shared" si="2"/>
         <v>6.7368895552787078E-3</v>
       </c>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="16"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
-      <c r="AF14" s="16"/>
-      <c r="AG14" s="16"/>
-      <c r="AH14" s="16"/>
-      <c r="AI14" s="16"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="10"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+      <c r="AH14" s="10"/>
+      <c r="AI14" s="10"/>
     </row>
     <row r="15" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
@@ -1945,33 +1982,33 @@
       <c r="Q15" s="1">
         <v>14892</v>
       </c>
-      <c r="R15" s="21">
+      <c r="R15" s="15">
         <v>109059</v>
       </c>
-      <c r="S15" s="22">
+      <c r="S15" s="16">
         <v>1839106</v>
       </c>
-      <c r="T15" s="20">
+      <c r="T15" s="14">
         <v>82643.12</v>
       </c>
-      <c r="U15" s="20">
+      <c r="U15" s="14">
         <f t="shared" si="0"/>
         <v>22.253588683486299</v>
       </c>
-      <c r="V15" s="18">
+      <c r="V15" s="12">
         <f t="shared" si="1"/>
         <v>1.319637980753873</v>
       </c>
-      <c r="W15" s="19">
+      <c r="W15" s="13">
         <f t="shared" si="2"/>
         <v>5.9300007721142772E-2</v>
       </c>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="16"/>
-      <c r="AD15" s="17"/>
-      <c r="AE15" s="15"/>
-      <c r="AF15" s="16"/>
-      <c r="AG15" s="16"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="10"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
     </row>
     <row r="16" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -2025,36 +2062,36 @@
       <c r="Q16" s="1">
         <v>111073</v>
       </c>
-      <c r="R16" s="21">
+      <c r="R16" s="15">
         <v>306748</v>
       </c>
-      <c r="S16" s="22">
+      <c r="S16" s="16">
         <v>12671469</v>
       </c>
-      <c r="T16" s="20">
+      <c r="T16" s="14">
         <v>55518.93</v>
       </c>
-      <c r="U16" s="20">
+      <c r="U16" s="14">
         <f t="shared" si="0"/>
         <v>228.23690946493386</v>
       </c>
-      <c r="V16" s="18">
+      <c r="V16" s="12">
         <f t="shared" si="1"/>
         <v>5.5251064816991251</v>
       </c>
-      <c r="W16" s="19">
+      <c r="W16" s="13">
         <f t="shared" si="2"/>
         <v>2.4207769438571013E-2</v>
       </c>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="16"/>
-      <c r="AC16" s="15"/>
-      <c r="AD16" s="15"/>
-      <c r="AE16" s="15"/>
-      <c r="AF16" s="16"/>
-      <c r="AG16" s="16"/>
-      <c r="AH16" s="16"/>
-      <c r="AI16" s="16"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="10"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="10"/>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="10"/>
+      <c r="AI16" s="10"/>
     </row>
     <row r="17" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -2108,36 +2145,36 @@
       <c r="Q17" s="1">
         <v>66136</v>
       </c>
-      <c r="R17" s="21">
+      <c r="R17" s="15">
         <v>203045</v>
       </c>
-      <c r="S17" s="22">
+      <c r="S17" s="16">
         <v>6805985</v>
       </c>
-      <c r="T17" s="20">
+      <c r="T17" s="14">
         <v>35826.11</v>
       </c>
-      <c r="U17" s="20">
+      <c r="U17" s="14">
         <f t="shared" si="0"/>
         <v>189.97276009033635</v>
       </c>
-      <c r="V17" s="18">
+      <c r="V17" s="12">
         <f t="shared" si="1"/>
         <v>5.6675145585161211</v>
       </c>
-      <c r="W17" s="19">
+      <c r="W17" s="13">
         <f t="shared" si="2"/>
         <v>2.9833301131283716E-2</v>
       </c>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="16"/>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="15"/>
-      <c r="AF17" s="16"/>
-      <c r="AG17" s="16"/>
-      <c r="AH17" s="16"/>
-      <c r="AI17" s="16"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="10"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10"/>
     </row>
     <row r="18" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -2191,35 +2228,35 @@
       <c r="Q18" s="1">
         <v>28242</v>
       </c>
-      <c r="R18" s="21">
+      <c r="R18" s="15">
         <v>235669</v>
       </c>
-      <c r="S18" s="22">
+      <c r="S18" s="16">
         <v>3190369</v>
       </c>
-      <c r="T18" s="20">
+      <c r="T18" s="14">
         <v>55857.13</v>
       </c>
-      <c r="U18" s="20">
+      <c r="U18" s="14">
         <f t="shared" si="0"/>
         <v>57.116593709701881</v>
       </c>
-      <c r="V18" s="18">
+      <c r="V18" s="12">
         <f t="shared" si="1"/>
         <v>4.2191390785742122</v>
       </c>
-      <c r="W18" s="19">
+      <c r="W18" s="13">
         <f t="shared" si="2"/>
         <v>7.3868884759098405E-2</v>
       </c>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="16"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="16"/>
-      <c r="AG18" s="16"/>
-      <c r="AI18" s="16"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="10"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="10"/>
+      <c r="AI18" s="10"/>
     </row>
     <row r="19" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -2273,35 +2310,35 @@
       <c r="Q19" s="1">
         <v>31681</v>
       </c>
-      <c r="R19" s="21">
+      <c r="R19" s="15">
         <v>286087</v>
       </c>
-      <c r="S19" s="22">
+      <c r="S19" s="16">
         <v>2937880</v>
       </c>
-      <c r="T19" s="20">
+      <c r="T19" s="14">
         <v>81758.720000000001</v>
       </c>
-      <c r="U19" s="20">
+      <c r="U19" s="14">
         <f t="shared" si="0"/>
         <v>35.933537119954913</v>
       </c>
-      <c r="V19" s="18">
+      <c r="V19" s="12">
         <f t="shared" si="1"/>
         <v>3.4991619242571312</v>
       </c>
-      <c r="W19" s="19">
+      <c r="W19" s="13">
         <f t="shared" si="2"/>
         <v>9.7378722071697954E-2</v>
       </c>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="16"/>
-      <c r="AC19" s="15"/>
-      <c r="AD19" s="15"/>
-      <c r="AE19" s="15"/>
-      <c r="AF19" s="16"/>
-      <c r="AG19" s="16"/>
-      <c r="AI19" s="16"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="10"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
+      <c r="AI19" s="10"/>
     </row>
     <row r="20" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -2355,35 +2392,35 @@
       <c r="Q20" s="1">
         <v>32989</v>
       </c>
-      <c r="R20" s="21">
+      <c r="R20" s="15">
         <v>167145</v>
       </c>
-      <c r="S20" s="22">
+      <c r="S20" s="16">
         <v>4505836</v>
       </c>
-      <c r="T20" s="20">
+      <c r="T20" s="14">
         <v>39486.339999999997</v>
       </c>
-      <c r="U20" s="20">
+      <c r="U20" s="14">
         <f t="shared" si="0"/>
         <v>114.1112597419766</v>
       </c>
-      <c r="V20" s="18">
+      <c r="V20" s="12">
         <f t="shared" si="1"/>
         <v>4.2329828492587565</v>
       </c>
-      <c r="W20" s="19">
+      <c r="W20" s="13">
         <f t="shared" si="2"/>
         <v>3.7095224948267093E-2</v>
       </c>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="16"/>
-      <c r="AC20" s="15"/>
-      <c r="AD20" s="15"/>
-      <c r="AE20" s="15"/>
-      <c r="AF20" s="16"/>
-      <c r="AG20" s="16"/>
-      <c r="AI20" s="16"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="10"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AI20" s="10"/>
     </row>
     <row r="21" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
@@ -2437,35 +2474,35 @@
       <c r="Q21" s="1">
         <v>48381</v>
       </c>
-      <c r="R21" s="21">
+      <c r="R21" s="15">
         <v>134135</v>
       </c>
-      <c r="S21" s="22">
+      <c r="S21" s="16">
         <v>4657757</v>
       </c>
-      <c r="T21" s="20">
+      <c r="T21" s="14">
         <v>43203.9</v>
       </c>
-      <c r="U21" s="20">
+      <c r="U21" s="14">
         <f t="shared" si="0"/>
         <v>107.80871634273757</v>
       </c>
-      <c r="V21" s="18">
+      <c r="V21" s="12">
         <f t="shared" si="1"/>
         <v>3.1046965667451318</v>
       </c>
-      <c r="W21" s="19">
+      <c r="W21" s="13">
         <f t="shared" si="2"/>
         <v>2.8798196213327572E-2</v>
       </c>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="16"/>
-      <c r="AC21" s="15"/>
-      <c r="AD21" s="15"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="16"/>
-      <c r="AG21" s="16"/>
-      <c r="AI21" s="16"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="10"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AI21" s="10"/>
     </row>
     <row r="22" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -2519,35 +2556,35 @@
       <c r="Q22" s="1">
         <v>6895</v>
       </c>
-      <c r="R22" s="21">
+      <c r="R22" s="15">
         <v>46801</v>
       </c>
-      <c r="S22" s="22">
+      <c r="S22" s="16">
         <v>1362359</v>
       </c>
-      <c r="T22" s="20">
+      <c r="T22" s="14">
         <v>30842.92</v>
       </c>
-      <c r="U22" s="20">
+      <c r="U22" s="14">
         <f t="shared" si="0"/>
         <v>44.170882653134015</v>
       </c>
-      <c r="V22" s="18">
+      <c r="V22" s="12">
         <f t="shared" si="1"/>
         <v>1.5173984823745612</v>
       </c>
-      <c r="W22" s="19">
+      <c r="W22" s="13">
         <f t="shared" si="2"/>
         <v>3.4352912851898801E-2</v>
       </c>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="16"/>
-      <c r="AC22" s="15"/>
-      <c r="AD22" s="15"/>
-      <c r="AE22" s="15"/>
-      <c r="AF22" s="16"/>
-      <c r="AG22" s="16"/>
-      <c r="AI22" s="16"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="10"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AI22" s="10"/>
     </row>
     <row r="23" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
@@ -2601,35 +2638,35 @@
       <c r="Q23" s="1">
         <v>43195</v>
       </c>
-      <c r="R23" s="21">
+      <c r="R23" s="15">
         <v>71244</v>
       </c>
-      <c r="S23" s="22">
+      <c r="S23" s="16">
         <v>6165129</v>
       </c>
-      <c r="T23" s="20">
+      <c r="T23" s="14">
         <v>9707.24</v>
       </c>
-      <c r="U23" s="20">
+      <c r="U23" s="14">
         <f t="shared" si="0"/>
         <v>635.10627119552009</v>
       </c>
-      <c r="V23" s="18">
+      <c r="V23" s="12">
         <f t="shared" si="1"/>
         <v>7.339264301696466</v>
       </c>
-      <c r="W23" s="19">
+      <c r="W23" s="13">
         <f t="shared" si="2"/>
         <v>1.1555962575965563E-2</v>
       </c>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="16"/>
-      <c r="AC23" s="15"/>
-      <c r="AD23" s="15"/>
-      <c r="AE23" s="15"/>
-      <c r="AF23" s="16"/>
-      <c r="AG23" s="16"/>
-      <c r="AI23" s="16"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="10"/>
+      <c r="AC23" s="9"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="10"/>
+      <c r="AG23" s="10"/>
+      <c r="AI23" s="10"/>
     </row>
     <row r="24" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -2683,35 +2720,35 @@
       <c r="Q24" s="1">
         <v>65239</v>
       </c>
-      <c r="R24" s="21">
+      <c r="R24" s="15">
         <v>77804</v>
       </c>
-      <c r="S24" s="22">
+      <c r="S24" s="16">
         <v>6984723</v>
       </c>
-      <c r="T24" s="20">
+      <c r="T24" s="14">
         <v>7800.06</v>
       </c>
-      <c r="U24" s="20">
+      <c r="U24" s="14">
         <f t="shared" si="0"/>
         <v>895.47041945831177</v>
       </c>
-      <c r="V24" s="18">
+      <c r="V24" s="12">
         <f t="shared" si="1"/>
         <v>9.9747950656789808</v>
       </c>
-      <c r="W24" s="19">
+      <c r="W24" s="13">
         <f t="shared" si="2"/>
         <v>1.1139167580446641E-2</v>
       </c>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="16"/>
-      <c r="AC24" s="15"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="15"/>
-      <c r="AF24" s="16"/>
-      <c r="AG24" s="16"/>
-      <c r="AI24" s="16"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="10"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="10"/>
+      <c r="AG24" s="10"/>
+      <c r="AI24" s="10"/>
     </row>
     <row r="25" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
@@ -2765,35 +2802,35 @@
       <c r="Q25" s="1">
         <v>85869</v>
       </c>
-      <c r="R25" s="21">
+      <c r="R25" s="15">
         <v>256295</v>
       </c>
-      <c r="S25" s="22">
+      <c r="S25" s="16">
         <v>10050811</v>
       </c>
-      <c r="T25" s="20">
+      <c r="T25" s="14">
         <v>56538.9</v>
       </c>
-      <c r="U25" s="20">
+      <c r="U25" s="14">
         <f t="shared" si="0"/>
         <v>177.76806764899919</v>
       </c>
-      <c r="V25" s="18">
+      <c r="V25" s="12">
         <f t="shared" si="1"/>
         <v>4.5330736890883978</v>
       </c>
-      <c r="W25" s="19">
+      <c r="W25" s="13">
         <f t="shared" si="2"/>
         <v>2.5499932294020852E-2</v>
       </c>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="16"/>
-      <c r="AC25" s="15"/>
-      <c r="AD25" s="15"/>
-      <c r="AE25" s="15"/>
-      <c r="AF25" s="16"/>
-      <c r="AG25" s="16"/>
-      <c r="AI25" s="16"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="10"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="10"/>
+      <c r="AG25" s="10"/>
+      <c r="AI25" s="10"/>
     </row>
     <row r="26" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -2847,36 +2884,36 @@
       <c r="Q26" s="1">
         <v>51787</v>
       </c>
-      <c r="R26" s="21">
+      <c r="R26" s="15">
         <v>291814</v>
       </c>
-      <c r="S26" s="22">
+      <c r="S26" s="16">
         <v>5707390</v>
       </c>
-      <c r="T26" s="20">
+      <c r="T26" s="14">
         <v>79626.740000000005</v>
       </c>
-      <c r="U26" s="20">
+      <c r="U26" s="14">
         <f t="shared" si="0"/>
         <v>71.676801034426376</v>
       </c>
-      <c r="V26" s="18">
+      <c r="V26" s="12">
         <f t="shared" si="1"/>
         <v>3.664773918912164</v>
       </c>
-      <c r="W26" s="19">
+      <c r="W26" s="13">
         <f t="shared" si="2"/>
         <v>5.112915010188545E-2</v>
       </c>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="16"/>
-      <c r="AC26" s="15"/>
-      <c r="AD26" s="15"/>
-      <c r="AE26" s="15"/>
-      <c r="AF26" s="16"/>
-      <c r="AG26" s="16"/>
-      <c r="AH26" s="16"/>
-      <c r="AI26" s="16"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="10"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="10"/>
+      <c r="AG26" s="10"/>
+      <c r="AH26" s="10"/>
+      <c r="AI26" s="10"/>
     </row>
     <row r="27" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -2930,35 +2967,35 @@
       <c r="Q27" s="1">
         <v>28880</v>
       </c>
-      <c r="R27" s="21">
+      <c r="R27" s="15">
         <v>162160</v>
       </c>
-      <c r="S27" s="22">
+      <c r="S27" s="16">
         <v>2961279</v>
       </c>
-      <c r="T27" s="20">
+      <c r="T27" s="14">
         <v>46923.27</v>
       </c>
-      <c r="U27" s="20">
+      <c r="U27" s="14">
         <f t="shared" si="0"/>
         <v>63.108964912291924</v>
       </c>
-      <c r="V27" s="18">
+      <c r="V27" s="12">
         <f t="shared" si="1"/>
         <v>3.4558546324670045</v>
       </c>
-      <c r="W27" s="19">
+      <c r="W27" s="13">
         <f t="shared" si="2"/>
         <v>5.476012223096844E-2</v>
       </c>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="16"/>
-      <c r="AC27" s="15"/>
-      <c r="AD27" s="15"/>
-      <c r="AE27" s="15"/>
-      <c r="AF27" s="16"/>
-      <c r="AG27" s="16"/>
-      <c r="AI27" s="16"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="10"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AI27" s="10"/>
     </row>
     <row r="28" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -3012,36 +3049,36 @@
       <c r="Q28" s="1">
         <v>57334</v>
       </c>
-      <c r="R28" s="21">
+      <c r="R28" s="15">
         <v>278101</v>
       </c>
-      <c r="S28" s="22">
+      <c r="S28" s="16">
         <v>6168187</v>
       </c>
-      <c r="T28" s="20">
+      <c r="T28" s="14">
         <v>68741.52</v>
       </c>
-      <c r="U28" s="20">
+      <c r="U28" s="14">
         <f t="shared" si="0"/>
         <v>89.730151442679755</v>
       </c>
-      <c r="V28" s="18">
+      <c r="V28" s="12">
         <f t="shared" si="1"/>
         <v>4.0456044614666649</v>
       </c>
-      <c r="W28" s="19">
+      <c r="W28" s="13">
         <f t="shared" si="2"/>
         <v>4.5086343847876208E-2</v>
       </c>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="16"/>
-      <c r="AC28" s="15"/>
-      <c r="AD28" s="15"/>
-      <c r="AE28" s="15"/>
-      <c r="AF28" s="16"/>
-      <c r="AG28" s="16"/>
-      <c r="AH28" s="16"/>
-      <c r="AI28" s="16"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="10"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="10"/>
+      <c r="AG28" s="10"/>
+      <c r="AH28" s="10"/>
+      <c r="AI28" s="10"/>
     </row>
     <row r="29" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
@@ -3095,35 +3132,35 @@
       <c r="Q29" s="1">
         <v>9115</v>
       </c>
-      <c r="R29" s="21">
+      <c r="R29" s="15">
         <v>150133</v>
       </c>
-      <c r="S29" s="22">
+      <c r="S29" s="16">
         <v>1084225</v>
       </c>
-      <c r="T29" s="20">
+      <c r="T29" s="14">
         <v>145545.79999999999</v>
       </c>
-      <c r="U29" s="20">
+      <c r="U29" s="14">
         <f t="shared" si="0"/>
         <v>7.4493733244105984</v>
       </c>
-      <c r="V29" s="18">
+      <c r="V29" s="12">
         <f t="shared" si="1"/>
         <v>1.0315172268797863</v>
       </c>
-      <c r="W29" s="19">
+      <c r="W29" s="13">
         <f t="shared" si="2"/>
         <v>0.13847033595425304</v>
       </c>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="16"/>
-      <c r="AC29" s="15"/>
-      <c r="AD29" s="15"/>
-      <c r="AE29" s="15"/>
-      <c r="AF29" s="16"/>
-      <c r="AG29" s="16"/>
-      <c r="AI29" s="16"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="10"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="10"/>
+      <c r="AG29" s="10"/>
+      <c r="AI29" s="10"/>
     </row>
     <row r="30" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
@@ -3177,35 +3214,35 @@
       <c r="Q30" s="1">
         <v>17786</v>
       </c>
-      <c r="R30" s="21">
+      <c r="R30" s="15">
         <v>194080</v>
       </c>
-      <c r="S30" s="22">
+      <c r="S30" s="16">
         <v>1961504</v>
       </c>
-      <c r="T30" s="20">
+      <c r="T30" s="14">
         <v>76824.17</v>
       </c>
-      <c r="U30" s="20">
+      <c r="U30" s="14">
         <f t="shared" si="0"/>
         <v>25.532381280526689</v>
       </c>
-      <c r="V30" s="18">
+      <c r="V30" s="12">
         <f t="shared" si="1"/>
         <v>2.5262882762026586</v>
       </c>
-      <c r="W30" s="19">
+      <c r="W30" s="13">
         <f t="shared" si="2"/>
         <v>9.89444834168067E-2</v>
       </c>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="16"/>
-      <c r="AC30" s="15"/>
-      <c r="AD30" s="15"/>
-      <c r="AE30" s="15"/>
-      <c r="AF30" s="16"/>
-      <c r="AG30" s="16"/>
-      <c r="AI30" s="16"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="10"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9"/>
+      <c r="AF30" s="10"/>
+      <c r="AG30" s="10"/>
+      <c r="AI30" s="10"/>
     </row>
     <row r="31" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
@@ -3259,36 +3296,36 @@
       <c r="Q31" s="1">
         <v>24802</v>
       </c>
-      <c r="R31" s="21">
+      <c r="R31" s="15">
         <v>100941</v>
       </c>
-      <c r="S31" s="22">
+      <c r="S31" s="16">
         <v>3104614</v>
       </c>
-      <c r="T31" s="20">
+      <c r="T31" s="14">
         <v>109781.18</v>
       </c>
-      <c r="U31" s="20">
+      <c r="U31" s="14">
         <f t="shared" si="0"/>
         <v>28.280020309492031</v>
       </c>
-      <c r="V31" s="18">
+      <c r="V31" s="12">
         <f t="shared" si="1"/>
         <v>0.91947454017163965</v>
       </c>
-      <c r="W31" s="19">
+      <c r="W31" s="13">
         <f t="shared" si="2"/>
         <v>3.2513220645143004E-2</v>
       </c>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="16"/>
-      <c r="AC31" s="15"/>
-      <c r="AD31" s="15"/>
-      <c r="AE31" s="15"/>
-      <c r="AF31" s="16"/>
-      <c r="AG31" s="16"/>
-      <c r="AH31" s="16"/>
-      <c r="AI31" s="16"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="10"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="10"/>
+      <c r="AH31" s="10"/>
+      <c r="AI31" s="10"/>
     </row>
     <row r="32" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
@@ -3342,36 +3379,36 @@
       <c r="Q32" s="1">
         <v>10861</v>
       </c>
-      <c r="R32" s="21">
+      <c r="R32" s="15">
         <v>33448</v>
       </c>
-      <c r="S32" s="22">
+      <c r="S32" s="16">
         <v>1377529</v>
       </c>
-      <c r="T32" s="20">
+      <c r="T32" s="14">
         <v>8952.65</v>
       </c>
-      <c r="U32" s="20">
+      <c r="U32" s="14">
         <f t="shared" si="0"/>
         <v>153.86829597940275</v>
       </c>
-      <c r="V32" s="18">
+      <c r="V32" s="12">
         <f t="shared" si="1"/>
         <v>3.7361004842141714</v>
       </c>
-      <c r="W32" s="19">
+      <c r="W32" s="13">
         <f t="shared" si="2"/>
         <v>2.4281158509185649E-2</v>
       </c>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="16"/>
-      <c r="AC32" s="15"/>
-      <c r="AD32" s="15"/>
-      <c r="AE32" s="15"/>
-      <c r="AF32" s="16"/>
-      <c r="AG32" s="16"/>
-      <c r="AH32" s="16"/>
-      <c r="AI32" s="16"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="10"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="10"/>
+      <c r="AH32" s="10"/>
+      <c r="AI32" s="10"/>
     </row>
     <row r="33" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
@@ -3425,36 +3462,36 @@
       <c r="Q33" s="1">
         <v>73892</v>
       </c>
-      <c r="R33" s="21">
+      <c r="R33" s="15">
         <v>85191</v>
       </c>
-      <c r="S33" s="22">
+      <c r="S33" s="16">
         <v>9267130</v>
       </c>
-      <c r="T33" s="20">
+      <c r="T33" s="14">
         <v>7354.22</v>
       </c>
-      <c r="U33" s="20">
+      <c r="U33" s="14">
         <f t="shared" si="0"/>
         <v>1260.1105215780872</v>
       </c>
-      <c r="V33" s="18">
+      <c r="V33" s="12">
         <f t="shared" si="1"/>
         <v>11.583961317447669</v>
       </c>
-      <c r="W33" s="19">
+      <c r="W33" s="13">
         <f t="shared" si="2"/>
         <v>9.1928137406079337E-3</v>
       </c>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="16"/>
-      <c r="AC33" s="15"/>
-      <c r="AD33" s="15"/>
-      <c r="AE33" s="15"/>
-      <c r="AF33" s="16"/>
-      <c r="AG33" s="16"/>
-      <c r="AH33" s="16"/>
-      <c r="AI33" s="16"/>
+      <c r="X33" s="9"/>
+      <c r="Y33" s="10"/>
+      <c r="AC33" s="9"/>
+      <c r="AD33" s="9"/>
+      <c r="AE33" s="9"/>
+      <c r="AF33" s="10"/>
+      <c r="AG33" s="10"/>
+      <c r="AH33" s="10"/>
+      <c r="AI33" s="10"/>
     </row>
     <row r="34" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
@@ -3508,35 +3545,35 @@
       <c r="Q34" s="1">
         <v>24959</v>
       </c>
-      <c r="R34" s="21">
+      <c r="R34" s="15">
         <v>150747</v>
       </c>
-      <c r="S34" s="22">
+      <c r="S34" s="16">
         <v>2117522</v>
       </c>
-      <c r="T34" s="20">
+      <c r="T34" s="14">
         <v>121298.15</v>
       </c>
-      <c r="U34" s="20">
+      <c r="U34" s="14">
         <f t="shared" si="0"/>
         <v>17.457166494295254</v>
       </c>
-      <c r="V34" s="18">
+      <c r="V34" s="12">
         <f t="shared" si="1"/>
         <v>1.2427807019315629</v>
       </c>
-      <c r="W34" s="19">
+      <c r="W34" s="13">
         <f t="shared" si="2"/>
         <v>7.1190287515312714E-2</v>
       </c>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="16"/>
-      <c r="AC34" s="15"/>
-      <c r="AD34" s="15"/>
-      <c r="AE34" s="15"/>
-      <c r="AF34" s="16"/>
-      <c r="AG34" s="16"/>
-      <c r="AI34" s="16"/>
+      <c r="X34" s="9"/>
+      <c r="Y34" s="10"/>
+      <c r="AC34" s="9"/>
+      <c r="AD34" s="9"/>
+      <c r="AE34" s="9"/>
+      <c r="AF34" s="10"/>
+      <c r="AG34" s="10"/>
+      <c r="AI34" s="10"/>
     </row>
     <row r="35" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
@@ -3590,35 +3627,35 @@
       <c r="Q35" s="1">
         <v>109770</v>
       </c>
-      <c r="R35" s="21">
+      <c r="R35" s="15">
         <v>240827</v>
       </c>
-      <c r="S35" s="22">
+      <c r="S35" s="16">
         <v>19835913</v>
       </c>
-      <c r="T35" s="20">
+      <c r="T35" s="14">
         <v>47126.400000000001</v>
       </c>
-      <c r="U35" s="20">
+      <c r="U35" s="14">
         <f t="shared" si="0"/>
         <v>420.90872631900589</v>
       </c>
-      <c r="V35" s="18">
+      <c r="V35" s="12">
         <f t="shared" si="1"/>
         <v>5.110235451891084</v>
       </c>
-      <c r="W35" s="19">
+      <c r="W35" s="13">
         <f t="shared" si="2"/>
         <v>1.214095867429949E-2</v>
       </c>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="16"/>
-      <c r="AC35" s="15"/>
-      <c r="AD35" s="15"/>
-      <c r="AE35" s="15"/>
-      <c r="AF35" s="16"/>
-      <c r="AG35" s="16"/>
-      <c r="AI35" s="16"/>
+      <c r="X35" s="9"/>
+      <c r="Y35" s="10"/>
+      <c r="AC35" s="9"/>
+      <c r="AD35" s="9"/>
+      <c r="AE35" s="9"/>
+      <c r="AF35" s="10"/>
+      <c r="AG35" s="10"/>
+      <c r="AI35" s="10"/>
     </row>
     <row r="36" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
@@ -3672,35 +3709,35 @@
       <c r="Q36" s="1">
         <v>93559</v>
       </c>
-      <c r="R36" s="21">
+      <c r="R36" s="15">
         <v>229902</v>
       </c>
-      <c r="S36" s="22">
+      <c r="S36" s="16">
         <v>10551162</v>
       </c>
-      <c r="T36" s="20">
+      <c r="T36" s="14">
         <v>48617.91</v>
       </c>
-      <c r="U36" s="20">
+      <c r="U36" s="14">
         <f t="shared" si="0"/>
         <v>217.02212209451207</v>
       </c>
-      <c r="V36" s="18">
+      <c r="V36" s="12">
         <f t="shared" si="1"/>
         <v>4.7287511947757519</v>
       </c>
-      <c r="W36" s="19">
+      <c r="W36" s="13">
         <f t="shared" si="2"/>
         <v>2.1789258851299981E-2</v>
       </c>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="16"/>
-      <c r="AC36" s="15"/>
-      <c r="AD36" s="15"/>
-      <c r="AE36" s="15"/>
-      <c r="AF36" s="16"/>
-      <c r="AG36" s="16"/>
-      <c r="AI36" s="16"/>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="10"/>
+      <c r="AC36" s="9"/>
+      <c r="AD36" s="9"/>
+      <c r="AE36" s="9"/>
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="10"/>
+      <c r="AI36" s="10"/>
     </row>
     <row r="37" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
@@ -3754,35 +3791,35 @@
       <c r="Q37" s="1">
         <v>6315</v>
       </c>
-      <c r="R37" s="21">
+      <c r="R37" s="15">
         <v>179369</v>
       </c>
-      <c r="S37" s="22">
+      <c r="S37" s="16">
         <v>779094</v>
       </c>
-      <c r="T37" s="20">
+      <c r="T37" s="14">
         <v>69000.800000000003</v>
       </c>
-      <c r="U37" s="20">
+      <c r="U37" s="14">
         <f t="shared" si="0"/>
         <v>11.291086480156752</v>
       </c>
-      <c r="V37" s="18">
+      <c r="V37" s="12">
         <f t="shared" si="1"/>
         <v>2.5995205852685763</v>
       </c>
-      <c r="W37" s="19">
+      <c r="W37" s="13">
         <f t="shared" si="2"/>
         <v>0.23022767470934188</v>
       </c>
-      <c r="X37" s="15"/>
-      <c r="Y37" s="16"/>
-      <c r="AC37" s="15"/>
-      <c r="AD37" s="15"/>
-      <c r="AE37" s="15"/>
-      <c r="AF37" s="16"/>
-      <c r="AG37" s="16"/>
-      <c r="AI37" s="16"/>
+      <c r="X37" s="9"/>
+      <c r="Y37" s="10"/>
+      <c r="AC37" s="9"/>
+      <c r="AD37" s="9"/>
+      <c r="AE37" s="9"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="10"/>
+      <c r="AI37" s="10"/>
     </row>
     <row r="38" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
@@ -3836,36 +3873,36 @@
       <c r="Q38" s="1">
         <v>107570</v>
       </c>
-      <c r="R38" s="21">
+      <c r="R38" s="15">
         <v>262465</v>
       </c>
-      <c r="S38" s="22">
+      <c r="S38" s="16">
         <v>11780017</v>
       </c>
-      <c r="T38" s="20">
+      <c r="T38" s="14">
         <v>40860.69</v>
       </c>
-      <c r="U38" s="20">
+      <c r="U38" s="14">
         <f t="shared" si="0"/>
         <v>288.29706497858945</v>
       </c>
-      <c r="V38" s="18">
+      <c r="V38" s="12">
         <f t="shared" si="1"/>
         <v>6.4234108626163673</v>
       </c>
-      <c r="W38" s="19">
+      <c r="W38" s="13">
         <f t="shared" si="2"/>
         <v>2.228052811808336E-2</v>
       </c>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="16"/>
-      <c r="AC38" s="15"/>
-      <c r="AD38" s="15"/>
-      <c r="AE38" s="15"/>
-      <c r="AF38" s="16"/>
-      <c r="AG38" s="16"/>
-      <c r="AH38" s="16"/>
-      <c r="AI38" s="16"/>
+      <c r="X38" s="9"/>
+      <c r="Y38" s="10"/>
+      <c r="AC38" s="9"/>
+      <c r="AD38" s="9"/>
+      <c r="AE38" s="9"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="10"/>
+      <c r="AH38" s="10"/>
+      <c r="AI38" s="10"/>
     </row>
     <row r="39" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
@@ -3919,36 +3956,36 @@
       <c r="Q39" s="1">
         <v>43076</v>
       </c>
-      <c r="R39" s="21">
+      <c r="R39" s="15">
         <v>239687</v>
       </c>
-      <c r="S39" s="22">
+      <c r="S39" s="16">
         <v>3959353</v>
       </c>
-      <c r="T39" s="20">
+      <c r="T39" s="14">
         <v>68594.92</v>
       </c>
-      <c r="U39" s="20">
+      <c r="U39" s="14">
         <f t="shared" si="0"/>
         <v>57.720790402554591</v>
       </c>
-      <c r="V39" s="18">
+      <c r="V39" s="12">
         <f t="shared" si="1"/>
         <v>3.4942383488456579</v>
       </c>
-      <c r="W39" s="19">
+      <c r="W39" s="13">
         <f t="shared" si="2"/>
         <v>6.0536910954895912E-2</v>
       </c>
-      <c r="X39" s="15"/>
-      <c r="Y39" s="16"/>
-      <c r="AC39" s="15"/>
-      <c r="AD39" s="15"/>
-      <c r="AE39" s="15"/>
-      <c r="AF39" s="16"/>
-      <c r="AG39" s="16"/>
-      <c r="AH39" s="16"/>
-      <c r="AI39" s="16"/>
+      <c r="X39" s="9"/>
+      <c r="Y39" s="10"/>
+      <c r="AC39" s="9"/>
+      <c r="AD39" s="9"/>
+      <c r="AE39" s="9"/>
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="10"/>
+      <c r="AH39" s="10"/>
+      <c r="AI39" s="10"/>
     </row>
     <row r="40" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
@@ -4002,33 +4039,33 @@
       <c r="Q40" s="1">
         <v>32544</v>
       </c>
-      <c r="R40" s="21">
+      <c r="R40" s="15">
         <v>161989</v>
       </c>
-      <c r="S40" s="22">
+      <c r="S40" s="16">
         <v>4237256</v>
       </c>
-      <c r="T40" s="20">
+      <c r="T40" s="14">
         <v>95988.01</v>
       </c>
-      <c r="U40" s="20">
+      <c r="U40" s="14">
         <f t="shared" si="0"/>
         <v>44.143596684627596</v>
       </c>
-      <c r="V40" s="18">
+      <c r="V40" s="12">
         <f t="shared" si="1"/>
         <v>1.6875961903991967</v>
       </c>
-      <c r="W40" s="19">
+      <c r="W40" s="13">
         <f t="shared" si="2"/>
         <v>3.8229693933998797E-2</v>
       </c>
-      <c r="X40" s="15"/>
-      <c r="Y40" s="16"/>
-      <c r="AD40" s="17"/>
-      <c r="AE40" s="15"/>
-      <c r="AF40" s="16"/>
-      <c r="AG40" s="16"/>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="10"/>
+      <c r="AD40" s="11"/>
+      <c r="AE40" s="9"/>
+      <c r="AF40" s="10"/>
+      <c r="AG40" s="10"/>
     </row>
     <row r="41" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
@@ -4082,35 +4119,35 @@
       <c r="Q41" s="1">
         <v>103551</v>
       </c>
-      <c r="R41" s="21">
+      <c r="R41" s="15">
         <v>252038</v>
       </c>
-      <c r="S41" s="22">
+      <c r="S41" s="16">
         <v>12964056</v>
       </c>
-      <c r="T41" s="20">
+      <c r="T41" s="14">
         <v>44742.7</v>
       </c>
-      <c r="U41" s="20">
+      <c r="U41" s="14">
         <f t="shared" si="0"/>
         <v>289.74684138418115</v>
       </c>
-      <c r="V41" s="18">
+      <c r="V41" s="12">
         <f t="shared" si="1"/>
         <v>5.633052989649709</v>
       </c>
-      <c r="W41" s="19">
+      <c r="W41" s="13">
         <f t="shared" si="2"/>
         <v>1.9441292138818282E-2</v>
       </c>
-      <c r="X41" s="15"/>
-      <c r="Y41" s="16"/>
-      <c r="AC41" s="15"/>
-      <c r="AD41" s="15"/>
-      <c r="AE41" s="15"/>
-      <c r="AF41" s="16"/>
-      <c r="AG41" s="16"/>
-      <c r="AI41" s="16"/>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="10"/>
+      <c r="AC41" s="9"/>
+      <c r="AD41" s="9"/>
+      <c r="AE41" s="9"/>
+      <c r="AF41" s="10"/>
+      <c r="AG41" s="10"/>
+      <c r="AI41" s="10"/>
     </row>
     <row r="42" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
@@ -4164,35 +4201,35 @@
       <c r="Q42" s="1">
         <v>9923</v>
       </c>
-      <c r="R42" s="21">
+      <c r="R42" s="15">
         <v>12737</v>
       </c>
-      <c r="S42" s="22">
+      <c r="S42" s="16">
         <v>1097379</v>
       </c>
-      <c r="T42" s="20">
+      <c r="T42" s="14">
         <v>1033.81</v>
       </c>
-      <c r="U42" s="20">
+      <c r="U42" s="14">
         <f t="shared" si="0"/>
         <v>1061.4900223445316</v>
       </c>
-      <c r="V42" s="18">
+      <c r="V42" s="12">
         <f t="shared" si="1"/>
         <v>12.320445729872995</v>
       </c>
-      <c r="W42" s="19">
+      <c r="W42" s="13">
         <f t="shared" si="2"/>
         <v>1.1606746620811953E-2</v>
       </c>
-      <c r="X42" s="15"/>
-      <c r="Y42" s="16"/>
-      <c r="AC42" s="15"/>
-      <c r="AD42" s="15"/>
-      <c r="AE42" s="15"/>
-      <c r="AF42" s="16"/>
-      <c r="AG42" s="16"/>
-      <c r="AI42" s="16"/>
+      <c r="X42" s="9"/>
+      <c r="Y42" s="10"/>
+      <c r="AC42" s="9"/>
+      <c r="AD42" s="9"/>
+      <c r="AE42" s="9"/>
+      <c r="AF42" s="10"/>
+      <c r="AG42" s="10"/>
+      <c r="AI42" s="10"/>
     </row>
     <row r="43" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
@@ -4246,36 +4283,36 @@
       <c r="Q43" s="1">
         <v>53758</v>
       </c>
-      <c r="R43" s="21">
+      <c r="R43" s="15">
         <v>166541</v>
       </c>
-      <c r="S43" s="22">
+      <c r="S43" s="16">
         <v>5190705</v>
       </c>
-      <c r="T43" s="20">
+      <c r="T43" s="14">
         <v>30060.7</v>
       </c>
-      <c r="U43" s="20">
+      <c r="U43" s="14">
         <f t="shared" si="0"/>
         <v>172.67412269175369</v>
       </c>
-      <c r="V43" s="18">
+      <c r="V43" s="12">
         <f t="shared" si="1"/>
         <v>5.540157082170408</v>
       </c>
-      <c r="W43" s="19">
+      <c r="W43" s="13">
         <f t="shared" si="2"/>
         <v>3.2084466368248632E-2</v>
       </c>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="16"/>
-      <c r="AC43" s="15"/>
-      <c r="AD43" s="15"/>
-      <c r="AE43" s="15"/>
-      <c r="AF43" s="16"/>
-      <c r="AG43" s="16"/>
-      <c r="AH43" s="16"/>
-      <c r="AI43" s="16"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="10"/>
+      <c r="AC43" s="9"/>
+      <c r="AD43" s="9"/>
+      <c r="AE43" s="9"/>
+      <c r="AF43" s="10"/>
+      <c r="AG43" s="10"/>
+      <c r="AH43" s="10"/>
+      <c r="AI43" s="10"/>
     </row>
     <row r="44" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
@@ -4329,35 +4366,35 @@
       <c r="Q44" s="1">
         <v>7243</v>
       </c>
-      <c r="R44" s="21">
+      <c r="R44" s="15">
         <v>166098</v>
       </c>
-      <c r="S44" s="22">
+      <c r="S44" s="16">
         <v>886667</v>
       </c>
-      <c r="T44" s="20">
+      <c r="T44" s="14">
         <v>75811</v>
       </c>
-      <c r="U44" s="20">
+      <c r="U44" s="14">
         <f t="shared" si="0"/>
         <v>11.695756552479192</v>
       </c>
-      <c r="V44" s="18">
+      <c r="V44" s="12">
         <f t="shared" si="1"/>
         <v>2.1909485430874147</v>
       </c>
-      <c r="W44" s="19">
+      <c r="W44" s="13">
         <f t="shared" si="2"/>
         <v>0.18732850100432294</v>
       </c>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="16"/>
-      <c r="AC44" s="15"/>
-      <c r="AD44" s="15"/>
-      <c r="AE44" s="15"/>
-      <c r="AF44" s="16"/>
-      <c r="AG44" s="16"/>
-      <c r="AI44" s="16"/>
+      <c r="X44" s="9"/>
+      <c r="Y44" s="10"/>
+      <c r="AC44" s="9"/>
+      <c r="AD44" s="9"/>
+      <c r="AE44" s="9"/>
+      <c r="AF44" s="10"/>
+      <c r="AG44" s="10"/>
+      <c r="AI44" s="10"/>
     </row>
     <row r="45" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
@@ -4411,33 +4448,33 @@
       <c r="Q45" s="1">
         <v>71484</v>
       </c>
-      <c r="R45" s="21">
+      <c r="R45" s="15">
         <v>203899</v>
       </c>
-      <c r="S45" s="22">
+      <c r="S45" s="16">
         <v>6975218</v>
       </c>
-      <c r="T45" s="20">
+      <c r="T45" s="14">
         <v>41234.9</v>
       </c>
-      <c r="U45" s="20">
+      <c r="U45" s="14">
         <f t="shared" si="0"/>
         <v>169.15811606187961</v>
       </c>
-      <c r="V45" s="18">
+      <c r="V45" s="12">
         <f t="shared" si="1"/>
         <v>4.9448161630075491</v>
       </c>
-      <c r="W45" s="19">
+      <c r="W45" s="13">
         <f t="shared" si="2"/>
         <v>2.9231917912816489E-2</v>
       </c>
-      <c r="X45" s="15"/>
-      <c r="Y45" s="16"/>
-      <c r="AD45" s="17"/>
-      <c r="AE45" s="15"/>
-      <c r="AF45" s="16"/>
-      <c r="AG45" s="16"/>
+      <c r="X45" s="9"/>
+      <c r="Y45" s="10"/>
+      <c r="AD45" s="11"/>
+      <c r="AE45" s="9"/>
+      <c r="AF45" s="10"/>
+      <c r="AG45" s="10"/>
     </row>
     <row r="46" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
@@ -4491,35 +4528,35 @@
       <c r="Q46" s="1">
         <v>258437</v>
       </c>
-      <c r="R46" s="21">
+      <c r="R46" s="15">
         <v>686281</v>
       </c>
-      <c r="S46" s="22">
+      <c r="S46" s="16">
         <v>29527941</v>
       </c>
-      <c r="T46" s="20">
+      <c r="T46" s="14">
         <v>261231.71</v>
       </c>
-      <c r="U46" s="20">
+      <c r="U46" s="14">
         <f t="shared" si="0"/>
         <v>113.03352491165793</v>
       </c>
-      <c r="V46" s="18">
+      <c r="V46" s="12">
         <f t="shared" si="1"/>
         <v>2.6270968405788104</v>
       </c>
-      <c r="W46" s="19">
+      <c r="W46" s="13">
         <f t="shared" si="2"/>
         <v>2.3241749229992028E-2</v>
       </c>
-      <c r="X46" s="15"/>
-      <c r="Y46" s="16"/>
-      <c r="AC46" s="15"/>
-      <c r="AD46" s="15"/>
-      <c r="AE46" s="15"/>
-      <c r="AF46" s="16"/>
-      <c r="AG46" s="16"/>
-      <c r="AI46" s="16"/>
+      <c r="X46" s="9"/>
+      <c r="Y46" s="10"/>
+      <c r="AC46" s="9"/>
+      <c r="AD46" s="9"/>
+      <c r="AE46" s="9"/>
+      <c r="AF46" s="10"/>
+      <c r="AG46" s="10"/>
+      <c r="AI46" s="10"/>
     </row>
     <row r="47" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
@@ -4573,36 +4610,36 @@
       <c r="Q47" s="1">
         <v>27916</v>
       </c>
-      <c r="R47" s="21">
+      <c r="R47" s="15">
         <v>102452</v>
       </c>
-      <c r="S47" s="22">
+      <c r="S47" s="16">
         <v>3271616</v>
       </c>
-      <c r="T47" s="20">
+      <c r="T47" s="14">
         <v>82169.62</v>
       </c>
-      <c r="U47" s="20">
+      <c r="U47" s="14">
         <f t="shared" si="0"/>
         <v>39.815396493253836</v>
       </c>
-      <c r="V47" s="18">
+      <c r="V47" s="12">
         <f t="shared" si="1"/>
         <v>1.2468355092794636</v>
       </c>
-      <c r="W47" s="19">
+      <c r="W47" s="13">
         <f t="shared" si="2"/>
         <v>3.1315411099591149E-2</v>
       </c>
-      <c r="X47" s="15"/>
-      <c r="Y47" s="16"/>
-      <c r="AC47" s="15"/>
-      <c r="AD47" s="15"/>
-      <c r="AE47" s="15"/>
-      <c r="AF47" s="16"/>
-      <c r="AG47" s="16"/>
-      <c r="AH47" s="16"/>
-      <c r="AI47" s="16"/>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="10"/>
+      <c r="AC47" s="9"/>
+      <c r="AD47" s="9"/>
+      <c r="AE47" s="9"/>
+      <c r="AF47" s="10"/>
+      <c r="AG47" s="10"/>
+      <c r="AH47" s="10"/>
+      <c r="AI47" s="10"/>
     </row>
     <row r="48" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
@@ -4656,36 +4693,36 @@
       <c r="Q48" s="1">
         <v>3200</v>
       </c>
-      <c r="R48" s="21">
+      <c r="R48" s="15">
         <v>29262</v>
       </c>
-      <c r="S48" s="22">
+      <c r="S48" s="16">
         <v>643077</v>
       </c>
-      <c r="T48" s="20">
+      <c r="T48" s="14">
         <v>9216.66</v>
       </c>
-      <c r="U48" s="20">
+      <c r="U48" s="14">
         <f t="shared" si="0"/>
         <v>69.773323525007982</v>
       </c>
-      <c r="V48" s="18">
+      <c r="V48" s="12">
         <f t="shared" si="1"/>
         <v>3.1749028389893952</v>
       </c>
-      <c r="W48" s="19">
+      <c r="W48" s="13">
         <f t="shared" si="2"/>
         <v>4.5503104604891792E-2</v>
       </c>
-      <c r="X48" s="15"/>
-      <c r="Y48" s="16"/>
-      <c r="AC48" s="15"/>
-      <c r="AD48" s="15"/>
-      <c r="AE48" s="15"/>
-      <c r="AF48" s="16"/>
-      <c r="AG48" s="16"/>
-      <c r="AH48" s="16"/>
-      <c r="AI48" s="16"/>
+      <c r="X48" s="9"/>
+      <c r="Y48" s="10"/>
+      <c r="AC48" s="9"/>
+      <c r="AD48" s="9"/>
+      <c r="AE48" s="9"/>
+      <c r="AF48" s="10"/>
+      <c r="AG48" s="10"/>
+      <c r="AH48" s="10"/>
+      <c r="AI48" s="10"/>
     </row>
     <row r="49" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
@@ -4739,36 +4776,36 @@
       <c r="Q49" s="1">
         <v>62623</v>
       </c>
-      <c r="R49" s="21">
+      <c r="R49" s="15">
         <v>164585</v>
       </c>
-      <c r="S49" s="22">
+      <c r="S49" s="16">
         <v>8642274</v>
       </c>
-      <c r="T49" s="20">
+      <c r="T49" s="14">
         <v>39490.089999999997</v>
       </c>
-      <c r="U49" s="20">
+      <c r="U49" s="14">
         <f t="shared" si="0"/>
         <v>218.84665241330168</v>
       </c>
-      <c r="V49" s="18">
+      <c r="V49" s="12">
         <f t="shared" si="1"/>
         <v>4.1677544923295953</v>
       </c>
-      <c r="W49" s="19">
+      <c r="W49" s="13">
         <f t="shared" si="2"/>
         <v>1.9044177493099616E-2</v>
       </c>
-      <c r="X49" s="15"/>
-      <c r="Y49" s="16"/>
-      <c r="AC49" s="15"/>
-      <c r="AD49" s="15"/>
-      <c r="AE49" s="15"/>
-      <c r="AF49" s="16"/>
-      <c r="AG49" s="16"/>
-      <c r="AH49" s="16"/>
-      <c r="AI49" s="16"/>
+      <c r="X49" s="9"/>
+      <c r="Y49" s="10"/>
+      <c r="AC49" s="9"/>
+      <c r="AD49" s="9"/>
+      <c r="AE49" s="9"/>
+      <c r="AF49" s="10"/>
+      <c r="AG49" s="10"/>
+      <c r="AH49" s="10"/>
+      <c r="AI49" s="10"/>
     </row>
     <row r="50" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
@@ -4822,36 +4859,36 @@
       <c r="Q50" s="1">
         <v>53789</v>
       </c>
-      <c r="R50" s="21">
+      <c r="R50" s="15">
         <v>168271</v>
       </c>
-      <c r="S50" s="22">
+      <c r="S50" s="16">
         <v>7738692</v>
       </c>
-      <c r="T50" s="20">
+      <c r="T50" s="14">
         <v>66455.520000000004</v>
       </c>
-      <c r="U50" s="20">
+      <c r="U50" s="14">
         <f t="shared" si="0"/>
         <v>116.44919789958756</v>
       </c>
-      <c r="V50" s="18">
+      <c r="V50" s="12">
         <f t="shared" si="1"/>
         <v>2.5320846184034069</v>
       </c>
-      <c r="W50" s="19">
+      <c r="W50" s="13">
         <f t="shared" si="2"/>
         <v>2.1744113863169642E-2</v>
       </c>
-      <c r="X50" s="15"/>
-      <c r="Y50" s="16"/>
-      <c r="AC50" s="15"/>
-      <c r="AD50" s="15"/>
-      <c r="AE50" s="15"/>
-      <c r="AF50" s="16"/>
-      <c r="AG50" s="16"/>
-      <c r="AH50" s="16"/>
-      <c r="AI50" s="16"/>
+      <c r="X50" s="9"/>
+      <c r="Y50" s="10"/>
+      <c r="AC50" s="9"/>
+      <c r="AD50" s="9"/>
+      <c r="AE50" s="9"/>
+      <c r="AF50" s="10"/>
+      <c r="AG50" s="10"/>
+      <c r="AH50" s="10"/>
+      <c r="AI50" s="10"/>
     </row>
     <row r="51" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
@@ -4905,33 +4942,33 @@
       <c r="Q51" s="1">
         <v>14463</v>
       </c>
-      <c r="R51" s="21">
+      <c r="R51" s="15">
         <v>80176</v>
       </c>
-      <c r="S51" s="22">
+      <c r="S51" s="16">
         <v>1793716</v>
       </c>
-      <c r="T51" s="20">
+      <c r="T51" s="14">
         <v>24038.21</v>
       </c>
-      <c r="U51" s="20">
+      <c r="U51" s="14">
         <f t="shared" si="0"/>
         <v>74.619366417050188</v>
       </c>
-      <c r="V51" s="18">
+      <c r="V51" s="12">
         <f t="shared" si="1"/>
         <v>3.3353565011704283</v>
       </c>
-      <c r="W51" s="19">
+      <c r="W51" s="13">
         <f t="shared" si="2"/>
         <v>4.4698268845235256E-2</v>
       </c>
-      <c r="X51" s="15"/>
-      <c r="Y51" s="16"/>
-      <c r="AD51" s="17"/>
-      <c r="AE51" s="15"/>
-      <c r="AF51" s="16"/>
-      <c r="AG51" s="16"/>
+      <c r="X51" s="9"/>
+      <c r="Y51" s="10"/>
+      <c r="AD51" s="11"/>
+      <c r="AE51" s="9"/>
+      <c r="AF51" s="10"/>
+      <c r="AG51" s="10"/>
     </row>
     <row r="52" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
@@ -4985,36 +5022,36 @@
       <c r="Q52" s="1">
         <v>53166</v>
       </c>
-      <c r="R52" s="21">
+      <c r="R52" s="15">
         <v>239526</v>
       </c>
-      <c r="S52" s="22">
+      <c r="S52" s="16">
         <v>5895908</v>
       </c>
-      <c r="T52" s="20">
+      <c r="T52" s="14">
         <v>54157.8</v>
       </c>
-      <c r="U52" s="20">
+      <c r="U52" s="14">
         <f t="shared" si="0"/>
         <v>108.86535272850817</v>
       </c>
-      <c r="V52" s="18">
+      <c r="V52" s="12">
         <f t="shared" si="1"/>
         <v>4.4227424304532308</v>
       </c>
-      <c r="W52" s="19">
+      <c r="W52" s="13">
         <f t="shared" si="2"/>
         <v>4.0625803523392831E-2</v>
       </c>
-      <c r="X52" s="15"/>
-      <c r="Y52" s="16"/>
-      <c r="AC52" s="15"/>
-      <c r="AD52" s="15"/>
-      <c r="AE52" s="15"/>
-      <c r="AF52" s="16"/>
-      <c r="AG52" s="16"/>
-      <c r="AH52" s="16"/>
-      <c r="AI52" s="16"/>
+      <c r="X52" s="9"/>
+      <c r="Y52" s="10"/>
+      <c r="AC52" s="9"/>
+      <c r="AD52" s="9"/>
+      <c r="AE52" s="9"/>
+      <c r="AF52" s="10"/>
+      <c r="AG52" s="10"/>
+      <c r="AH52" s="10"/>
+      <c r="AI52" s="10"/>
     </row>
     <row r="53" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
@@ -5068,35 +5105,35 @@
       <c r="Q53" s="1">
         <v>6387</v>
       </c>
-      <c r="R53" s="21">
+      <c r="R53" s="15">
         <v>62575</v>
       </c>
-      <c r="S53" s="22">
+      <c r="S53" s="16">
         <v>576851</v>
       </c>
-      <c r="T53" s="20">
+      <c r="T53" s="14">
         <v>97093.14</v>
       </c>
-      <c r="U53" s="20">
+      <c r="U53" s="14">
         <f t="shared" si="0"/>
         <v>5.9412127365537879</v>
       </c>
-      <c r="V53" s="18">
+      <c r="V53" s="12">
         <f t="shared" si="1"/>
         <v>0.6444842550153389</v>
       </c>
-      <c r="W53" s="19">
+      <c r="W53" s="13">
         <f t="shared" si="2"/>
         <v>0.10847688571225499</v>
       </c>
-      <c r="X53" s="15"/>
-      <c r="Y53" s="16"/>
-      <c r="AC53" s="15"/>
-      <c r="AD53" s="15"/>
-      <c r="AE53" s="15"/>
-      <c r="AF53" s="16"/>
-      <c r="AG53" s="16"/>
-      <c r="AI53" s="16"/>
+      <c r="X53" s="9"/>
+      <c r="Y53" s="10"/>
+      <c r="AC53" s="9"/>
+      <c r="AD53" s="9"/>
+      <c r="AE53" s="9"/>
+      <c r="AF53" s="10"/>
+      <c r="AG53" s="10"/>
+      <c r="AI53" s="10"/>
     </row>
     <row r="54" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
@@ -5150,92 +5187,131 @@
       <c r="Q54" s="6">
         <v>2782302</v>
       </c>
-      <c r="R54" s="23">
+      <c r="R54" s="17">
         <v>8790746</v>
       </c>
-      <c r="S54" s="22">
+      <c r="S54" s="16">
         <f>SUM(S3:S53)</f>
         <v>331700114</v>
       </c>
-      <c r="T54" s="20">
+      <c r="T54" s="14">
         <f>SUM(T3:T53)</f>
         <v>3531905.4399999995</v>
       </c>
-      <c r="U54" s="20">
+      <c r="U54" s="14">
         <f>S54/T54</f>
         <v>93.915343894371091</v>
       </c>
-      <c r="V54" s="18">
+      <c r="V54" s="12">
         <f>R54/T54</f>
         <v>2.4889528186235927</v>
       </c>
-      <c r="W54" s="19">
+      <c r="W54" s="13">
         <f t="shared" si="2"/>
         <v>2.650208917323435E-2</v>
       </c>
-      <c r="Y54" s="16"/>
-      <c r="AC54" s="15"/>
-      <c r="AD54" s="15"/>
-      <c r="AE54" s="15"/>
-      <c r="AF54" s="16"/>
-      <c r="AG54" s="16"/>
-      <c r="AH54" s="16"/>
-      <c r="AI54" s="16"/>
+      <c r="Y54" s="10"/>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="9"/>
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="10"/>
+      <c r="AG54" s="10"/>
+      <c r="AH54" s="10"/>
+      <c r="AI54" s="10"/>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="T55" s="15"/>
-      <c r="V55" s="16"/>
-      <c r="Y55" s="16"/>
-      <c r="AC55" s="15"/>
-      <c r="AD55" s="15"/>
-      <c r="AE55" s="15"/>
-      <c r="AF55" s="16"/>
-      <c r="AG55" s="16"/>
-      <c r="AH55" s="16"/>
-      <c r="AI55" s="16"/>
+      <c r="T55" s="9"/>
+      <c r="V55" s="10"/>
+      <c r="Y55" s="10"/>
+      <c r="AC55" s="9"/>
+      <c r="AD55" s="9"/>
+      <c r="AE55" s="9"/>
+      <c r="AF55" s="10"/>
+      <c r="AG55" s="10"/>
+      <c r="AH55" s="10"/>
+      <c r="AI55" s="10"/>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="Y56" s="16"/>
-      <c r="AC56" s="15"/>
-      <c r="AD56" s="15"/>
-      <c r="AE56" s="15"/>
-      <c r="AF56" s="16"/>
-      <c r="AG56" s="16"/>
-      <c r="AI56" s="16"/>
+      <c r="A56" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y56" s="10"/>
+      <c r="AC56" s="9"/>
+      <c r="AD56" s="9"/>
+      <c r="AE56" s="9"/>
+      <c r="AF56" s="10"/>
+      <c r="AG56" s="10"/>
+      <c r="AI56" s="10"/>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="T57" s="15"/>
-      <c r="V57" s="16"/>
-      <c r="Y57" s="16"/>
-      <c r="AC57" s="15"/>
-      <c r="AD57" s="15"/>
-      <c r="AE57" s="15"/>
-      <c r="AF57" s="16"/>
-      <c r="AG57" s="16"/>
-      <c r="AI57" s="16"/>
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="S57" t="s">
+        <v>73</v>
+      </c>
+      <c r="T57" s="9"/>
+      <c r="V57" s="10"/>
+      <c r="Y57">
+        <v>2020</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC57" s="9"/>
+      <c r="AD57" s="9"/>
+      <c r="AE57" s="9"/>
+      <c r="AF57" s="10"/>
+      <c r="AG57" s="10"/>
+      <c r="AI57" s="10"/>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="T58" s="15"/>
-      <c r="V58" s="16"/>
-      <c r="Y58" s="16"/>
-      <c r="AC58" s="15"/>
-      <c r="AD58" s="15"/>
-      <c r="AE58" s="15"/>
-      <c r="AF58" s="16"/>
-      <c r="AG58" s="16"/>
-      <c r="AI58" s="16"/>
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+      <c r="S58" t="s">
+        <v>76</v>
+      </c>
+      <c r="T58" s="9"/>
+      <c r="V58" s="10"/>
+      <c r="Y58" s="25">
+        <v>2021</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC58" s="9"/>
+      <c r="AD58" s="9"/>
+      <c r="AE58" s="9"/>
+      <c r="AF58" s="10"/>
+      <c r="AG58" s="10"/>
+      <c r="AI58" s="10"/>
+    </row>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="S59" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y59">
+        <v>2012</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="U1:U2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>